<commit_message>
extended functionality of io.saveMatches().Now it handles filters in file pattern
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_io.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_io.data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kg094044\IdeaProjects\nexial-core\src\test\resources\unittesting\artifact\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D56D4FA-61B7-B04F-93C0-C6CF5096945E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7A778D48-2EEC-4FF1-A3C3-9E49D1B1F4EB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9140" yWindow="-6840" windowWidth="33600" windowHeight="6840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9135" yWindow="-6840" windowWidth="33600" windowHeight="6840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
+    <sheet name="saveMatches" sheetId="4" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
     <definedName name="base">'[1]#system'!$B$2:$B$24</definedName>
@@ -36,7 +37,7 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>true</t>
   </si>
@@ -103,6 +104,48 @@
   </si>
   <si>
     <t>$(syspath|data|fullpath)/unitTest_io_filter1_expected.txt</t>
+  </si>
+  <si>
+    <t>fileDirectory</t>
+  </si>
+  <si>
+    <t>outputText</t>
+  </si>
+  <si>
+    <t>outputLog</t>
+  </si>
+  <si>
+    <t>outputTextFile1</t>
+  </si>
+  <si>
+    <t>outputLogFile1</t>
+  </si>
+  <si>
+    <t>outputLogFile2</t>
+  </si>
+  <si>
+    <t>outputTextFile2</t>
+  </si>
+  <si>
+    <t>${outputTextFile1},${outputTextFile2}</t>
+  </si>
+  <si>
+    <t>${outputLogFile1},${outputLogFile2}</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)\io_saveMatches</t>
+  </si>
+  <si>
+    <t>${fileDirectory}\unitTest_io_saveMatches1.txt</t>
+  </si>
+  <si>
+    <t>${fileDirectory}\unitTest_io_saveMatches2.txt</t>
+  </si>
+  <si>
+    <t>${fileDirectory}\unitTest_io_saveMatches3.json</t>
+  </si>
+  <si>
+    <t>${fileDirectory}\unitTest_io_saveMatches4.json</t>
   </si>
 </sst>
 </file>
@@ -197,7 +240,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -221,6 +264,10 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -231,7 +278,267 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -588,17 +895,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="56.83203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="27.875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="56.875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
-    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+    <col min="10" max="27" width="21.125" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.875" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
@@ -713,22 +1020,255 @@
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="4" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="24" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="23" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="22" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9 B12:B1048576">
-    <cfRule type="expression" dxfId="1" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56E3E307-7F2E-46DB-89A3-7D5088FF1029}">
+  <dimension ref="A1:AAA14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="27.875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="56.875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.125" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.875" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:703">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="1:703">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="1:703">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="HA3" s="6"/>
+      <c r="AAA3" s="6"/>
+    </row>
+    <row r="4" spans="1:703">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="1:703">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="HA5" s="4"/>
+      <c r="AAA5" s="5"/>
+    </row>
+    <row r="6" spans="1:703">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="1:703">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="1:703">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
+    </row>
+    <row r="9" spans="1:703">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:703">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:703">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:703">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:703">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="HA13" s="4"/>
+      <c r="AAA13" s="5"/>
+    </row>
+    <row r="14" spans="1:703">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="HA14" s="4"/>
+      <c r="AAA14" s="5"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A19:A1048576 A13:A17 A1:A8">
+    <cfRule type="beginsWith" dxfId="19" priority="16" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="18" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="17" priority="18" stopIfTrue="1">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:B17 B19:B1048576 B1:B8">
+    <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="15" priority="20">
+      <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18">
+    <cfRule type="beginsWith" dxfId="14" priority="11" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A18,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="13" priority="12" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A18,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="12" priority="13" stopIfTrue="1">
+      <formula>LEN(TRIM(A18))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18">
+    <cfRule type="expression" dxfId="11" priority="14" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="10" priority="15">
+      <formula>LEN(TRIM(B18))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:A11">
+    <cfRule type="beginsWith" dxfId="9" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A9,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="8" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A9,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8" stopIfTrue="1">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:B11">
+    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="10">
+      <formula>LEN(TRIM(B9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A12,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A12,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A12))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
+      <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[enhancement] - omit the creation of hyperlink on path longer than 254 characeter; Excel doesn't support long path.
[io]
- [`saveMatches(var,path,filePattern)`]: now support muti-criteria filtering using Nexial Filter syntax on file `name`, `size` and `lastMod`.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_io.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_io.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kg094044\IdeaProjects\nexial-core\src\test\resources\unittesting\artifact\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7A778D48-2EEC-4FF1-A3C3-9E49D1B1F4EB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A5339F-F026-9A4A-A323-7DB14B60406B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9135" yWindow="-6840" windowWidth="33600" windowHeight="6840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="10520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -37,15 +37,39 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={53CD440D-8BE8-A646-9E12-01222352B648}</author>
+  </authors>
+  <commentList>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{53CD440D-8BE8-A646-9E12-01222352B648}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Must explicitly use $(syspath) here so that Nexial can recognize these data variables as file paths</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
@@ -136,23 +160,23 @@
     <t>$(syspath|data|fullpath)\io_saveMatches</t>
   </si>
   <si>
-    <t>${fileDirectory}\unitTest_io_saveMatches1.txt</t>
-  </si>
-  <si>
-    <t>${fileDirectory}\unitTest_io_saveMatches2.txt</t>
-  </si>
-  <si>
-    <t>${fileDirectory}\unitTest_io_saveMatches3.json</t>
-  </si>
-  <si>
-    <t>${fileDirectory}\unitTest_io_saveMatches4.json</t>
+    <t>$(syspath|data|fullpath)\io_saveMatches\unitTest_io_saveMatches1.txt</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)\io_saveMatches\unitTest_io_saveMatches3.json</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)\io_saveMatches\unitTest_io_saveMatches4.json</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)\io_saveMatches\unitTest_io_saveMatches2.txt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -197,6 +221,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -628,6 +658,12 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Mike Liu" id="{A98EC98D-3EF7-EA4B-B035-7EFF28AD980C}" userId="61b9eb749b77dc95" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -891,6 +927,14 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B9" dT="2019-05-10T19:21:10.60" personId="{A98EC98D-3EF7-EA4B-B035-7EFF28AD980C}" id="{53CD440D-8BE8-A646-9E12-01222352B648}">
+    <text>Must explicitly use $(syspath) here so that Nexial can recognize these data variables as file paths</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA12"/>
@@ -899,13 +943,13 @@
       <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="27.875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="56.875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="27.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="56.83203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
-    <col min="10" max="27" width="21.125" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.875" style="3" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
@@ -1044,21 +1088,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56E3E307-7F2E-46DB-89A3-7D5088FF1029}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56E3E307-7F2E-46DB-89A3-7D5088FF1029}">
   <dimension ref="A1:AAA14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="27.875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="56.875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.125" style="3" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="27.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="84" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.1640625" style="3" customWidth="1" collapsed="1"/>
     <col min="4" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
-    <col min="10" max="27" width="21.125" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.875" style="3" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
@@ -1154,7 +1198,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:703">
@@ -1162,7 +1206,7 @@
         <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:703">
@@ -1170,7 +1214,7 @@
         <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:703">
@@ -1183,7 +1227,7 @@
       <c r="HA13" s="4"/>
       <c r="AAA13" s="5"/>
     </row>
-    <row r="14" spans="1:703">
+    <row r="14" spans="1:703" ht="18">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -1273,5 +1317,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[nexial interactive] - Option `L` to reload script file, data file and `project.properties` (option `L`)
[io]
- [`saveMatches(var,path,fileFilter,textFilter)`]: WAS `saveMatches(var,path,filePattern)`. This command has been enhanced to support content-level filtering (REGEX-based) so that in addition to filtering by file name, last modified date and file size, one can also filter files by its content (support all text file, PDF and XLSX). This command now also support recursively scanning.

Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_io.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_io.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A5339F-F026-9A4A-A323-7DB14B60406B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88369661-D4EF-7D45-8AE9-47A1668CDFE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="10520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="460" windowWidth="51200" windowHeight="10520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -71,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>true</t>
   </si>
@@ -157,26 +159,53 @@
     <t>${outputLogFile1},${outputLogFile2}</t>
   </si>
   <si>
-    <t>$(syspath|data|fullpath)\io_saveMatches</t>
-  </si>
-  <si>
-    <t>$(syspath|data|fullpath)\io_saveMatches\unitTest_io_saveMatches1.txt</t>
-  </si>
-  <si>
-    <t>$(syspath|data|fullpath)\io_saveMatches\unitTest_io_saveMatches3.json</t>
-  </si>
-  <si>
-    <t>$(syspath|data|fullpath)\io_saveMatches\unitTest_io_saveMatches4.json</t>
-  </si>
-  <si>
-    <t>$(syspath|data|fullpath)\io_saveMatches\unitTest_io_saveMatches2.txt</t>
+    <t>0</t>
+  </si>
+  <si>
+    <t>matchingPdfs1</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/io_saveMatches/unitTest_io_saveMatches2.txt</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/io_saveMatches</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/io_saveMatches/unitTest_io_saveMatches1.txt</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/io_saveMatches/unitTest_io_saveMatches3.json</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/io_saveMatches/unitTest_io_saveMatches4.json</t>
+  </si>
+  <si>
+    <t>matchingPdfs2</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/io_saveMatches/sample-1.pdf,$(syspath|data|fullpath)/io_saveMatches/sample-2.pdf,$(syspath|data|fullpath)/io_saveMatches/sample-4.pdf</t>
+  </si>
+  <si>
+    <t>matchingXlsx2</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/io_saveMatches/example-1.xlsx,$(syspath|data|fullpath)/io_saveMatches/example-2.xlsx</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/io_saveMatches/sample-3.pdf,$(syspath|data|fullpath)/io_saveMatches/subdir/sample-5.pdf</t>
+  </si>
+  <si>
+    <t>matchingPdfs3</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/io_saveMatches/sample-3.pdf,$(syspath|data|fullpath)/io_saveMatches/sample-1.pdf,$(syspath|data|fullpath)/io_saveMatches/subdir/sample-5.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -221,12 +250,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -308,7 +331,109 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="33">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -937,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA12"/>
+  <dimension ref="A1:AAA63"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17"/>
@@ -952,7 +1077,7 @@
     <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:703">
+    <row r="1" spans="1:703" ht="23" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -962,7 +1087,7 @@
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
-    <row r="2" spans="1:703">
+    <row r="2" spans="1:703" ht="23" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -972,7 +1097,7 @@
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
-    <row r="3" spans="1:703">
+    <row r="3" spans="1:703" ht="23" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -982,7 +1107,7 @@
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
     </row>
-    <row r="4" spans="1:703">
+    <row r="4" spans="1:703" ht="23" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -992,7 +1117,7 @@
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
-    <row r="5" spans="1:703">
+    <row r="5" spans="1:703" ht="23" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1002,7 +1127,7 @@
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
-    <row r="6" spans="1:703">
+    <row r="6" spans="1:703" ht="23" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1012,7 +1137,7 @@
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
-    <row r="7" spans="1:703">
+    <row r="7" spans="1:703" ht="23" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1022,7 +1147,7 @@
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
-    <row r="8" spans="1:703">
+    <row r="8" spans="1:703" ht="23" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1032,7 +1157,7 @@
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
-    <row r="9" spans="1:703">
+    <row r="9" spans="1:703" ht="23" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1042,7 +1167,7 @@
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>
-    <row r="10" spans="1:703">
+    <row r="10" spans="1:703" ht="23" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1052,33 +1177,84 @@
       <c r="HA10" s="4"/>
       <c r="AAA10" s="5"/>
     </row>
-    <row r="11" spans="1:703">
+    <row r="11" spans="1:703" ht="23" customHeight="1">
       <c r="B11" s="3"/>
       <c r="HA11" s="4"/>
       <c r="AAA11" s="5"/>
     </row>
-    <row r="12" spans="1:703">
+    <row r="12" spans="1:703" ht="23" customHeight="1">
       <c r="HA12" s="4"/>
       <c r="AAA12" s="5"/>
     </row>
+    <row r="13" spans="1:703" ht="23" customHeight="1"/>
+    <row r="14" spans="1:703" ht="23" customHeight="1"/>
+    <row r="15" spans="1:703" ht="23" customHeight="1"/>
+    <row r="16" spans="1:703" ht="23" customHeight="1"/>
+    <row r="17" ht="23" customHeight="1"/>
+    <row r="18" ht="23" customHeight="1"/>
+    <row r="19" ht="23" customHeight="1"/>
+    <row r="20" ht="23" customHeight="1"/>
+    <row r="21" ht="23" customHeight="1"/>
+    <row r="22" ht="23" customHeight="1"/>
+    <row r="23" ht="23" customHeight="1"/>
+    <row r="24" ht="23" customHeight="1"/>
+    <row r="25" ht="23" customHeight="1"/>
+    <row r="26" ht="23" customHeight="1"/>
+    <row r="27" ht="23" customHeight="1"/>
+    <row r="28" ht="23" customHeight="1"/>
+    <row r="29" ht="23" customHeight="1"/>
+    <row r="30" ht="23" customHeight="1"/>
+    <row r="31" ht="23" customHeight="1"/>
+    <row r="32" ht="23" customHeight="1"/>
+    <row r="33" ht="23" customHeight="1"/>
+    <row r="34" ht="23" customHeight="1"/>
+    <row r="35" ht="23" customHeight="1"/>
+    <row r="36" ht="23" customHeight="1"/>
+    <row r="37" ht="23" customHeight="1"/>
+    <row r="38" ht="23" customHeight="1"/>
+    <row r="39" ht="23" customHeight="1"/>
+    <row r="40" ht="23" customHeight="1"/>
+    <row r="41" ht="23" customHeight="1"/>
+    <row r="42" ht="23" customHeight="1"/>
+    <row r="43" ht="23" customHeight="1"/>
+    <row r="44" ht="23" customHeight="1"/>
+    <row r="45" ht="23" customHeight="1"/>
+    <row r="46" ht="23" customHeight="1"/>
+    <row r="47" ht="23" customHeight="1"/>
+    <row r="48" ht="23" customHeight="1"/>
+    <row r="49" ht="23" customHeight="1"/>
+    <row r="50" ht="23" customHeight="1"/>
+    <row r="51" ht="23" customHeight="1"/>
+    <row r="52" ht="23" customHeight="1"/>
+    <row r="53" ht="23" customHeight="1"/>
+    <row r="54" ht="23" customHeight="1"/>
+    <row r="55" ht="23" customHeight="1"/>
+    <row r="56" ht="23" customHeight="1"/>
+    <row r="57" ht="23" customHeight="1"/>
+    <row r="58" ht="23" customHeight="1"/>
+    <row r="59" ht="23" customHeight="1"/>
+    <row r="60" ht="23" customHeight="1"/>
+    <row r="61" ht="23" customHeight="1"/>
+    <row r="62" ht="23" customHeight="1"/>
+    <row r="63" ht="23" customHeight="1"/>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="24" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="32" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="23" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="31" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="22" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B9 B12:B1048576">
-    <cfRule type="expression" dxfId="21" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="20" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="10">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1089,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56E3E307-7F2E-46DB-89A3-7D5088FF1029}">
-  <dimension ref="A1:AAA14"/>
+  <dimension ref="A1:AAA30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17"/>
@@ -1105,7 +1281,7 @@
     <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:703">
+    <row r="1" spans="1:703" ht="23" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1115,7 +1291,7 @@
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
-    <row r="2" spans="1:703">
+    <row r="2" spans="1:703" ht="23" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1125,7 +1301,7 @@
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
-    <row r="3" spans="1:703">
+    <row r="3" spans="1:703" ht="23" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1135,17 +1311,17 @@
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
     </row>
-    <row r="4" spans="1:703">
+    <row r="4" spans="1:703" ht="23" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
-    <row r="5" spans="1:703">
+    <row r="5" spans="1:703" ht="23" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1155,7 +1331,7 @@
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
-    <row r="6" spans="1:703">
+    <row r="6" spans="1:703" ht="23" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -1165,7 +1341,7 @@
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
-    <row r="7" spans="1:703">
+    <row r="7" spans="1:703" ht="23" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1175,49 +1351,49 @@
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
-    <row r="8" spans="1:703">
+    <row r="8" spans="1:703" ht="23" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
-    <row r="9" spans="1:703">
+    <row r="9" spans="1:703" ht="23" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:703">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:703" ht="23" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:703">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:703" ht="23" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:703">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:703" ht="23" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:703">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:703" ht="23" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
@@ -1227,7 +1403,7 @@
       <c r="HA13" s="4"/>
       <c r="AAA13" s="5"/>
     </row>
-    <row r="14" spans="1:703" ht="18">
+    <row r="14" spans="1:703" ht="23" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -1237,82 +1413,145 @@
       <c r="HA14" s="4"/>
       <c r="AAA14" s="5"/>
     </row>
+    <row r="15" spans="1:703" ht="23" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:703" ht="23" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="23" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="23" customHeight="1">
+      <c r="A18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="23" customHeight="1"/>
+    <row r="20" spans="1:2" ht="23" customHeight="1"/>
+    <row r="21" spans="1:2" ht="23" customHeight="1"/>
+    <row r="22" spans="1:2" ht="23" customHeight="1"/>
+    <row r="23" spans="1:2" ht="23" customHeight="1"/>
+    <row r="24" spans="1:2" ht="23" customHeight="1"/>
+    <row r="25" spans="1:2" ht="23" customHeight="1"/>
+    <row r="26" spans="1:2" ht="23" customHeight="1"/>
+    <row r="27" spans="1:2" ht="23" customHeight="1"/>
+    <row r="28" spans="1:2" ht="23" customHeight="1"/>
+    <row r="29" spans="1:2" ht="23" customHeight="1"/>
+    <row r="30" spans="1:2" ht="23" customHeight="1"/>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A19:A1048576 A13:A17 A1:A8">
-    <cfRule type="beginsWith" dxfId="19" priority="16" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+  <conditionalFormatting sqref="A19:A1048576 A13:A15 A1:A8 A17">
+    <cfRule type="beginsWith" dxfId="27" priority="24" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="18" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="26" priority="25" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="17" priority="18" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="26" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:B17 B19:B1048576 B1:B8">
-    <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
+  <conditionalFormatting sqref="B14:B15 B19:B1048576 B1:B8 B17">
+    <cfRule type="expression" dxfId="24" priority="27" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="15" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="28">
       <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18">
+    <cfRule type="expression" dxfId="19" priority="22" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="18" priority="23">
+      <formula>LEN(TRIM(B18))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:A11">
+    <cfRule type="beginsWith" dxfId="17" priority="14" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A9,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="16" priority="15" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A9,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="15" priority="16" stopIfTrue="1">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:B11">
+    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="13" priority="18">
+      <formula>LEN(TRIM(B9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12">
+    <cfRule type="beginsWith" dxfId="12" priority="9" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A12,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="11" priority="10" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A12,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="10" priority="11" stopIfTrue="1">
+      <formula>LEN(TRIM(A12))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12">
+    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="8" priority="13">
+      <formula>LEN(TRIM(B12))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A16">
+    <cfRule type="beginsWith" dxfId="7" priority="4" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A16,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="6" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A16,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="6" stopIfTrue="1">
+      <formula>LEN(TRIM(A16))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16">
+    <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="3" priority="8">
+      <formula>LEN(TRIM(B16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18">
-    <cfRule type="beginsWith" dxfId="14" priority="11" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A18,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="12" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A18,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="12" priority="13" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A18))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="11" priority="14" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="15">
-      <formula>LEN(TRIM(B18))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A9:A11">
-    <cfRule type="beginsWith" dxfId="9" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
-      <formula>LEFT(A9,LEN("sentry.scope."))="sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
-      <formula>LEFT(A9,LEN("sentry."))="sentry."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="7" priority="8" stopIfTrue="1">
-      <formula>LEN(TRIM(A9))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9:B11">
-    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="10">
-      <formula>LEN(TRIM(B9))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A12">
-    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
-      <formula>LEFT(A12,LEN("sentry.scope."))="sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
-      <formula>LEFT(A12,LEN("sentry."))="sentry."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>LEN(TRIM(A12))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
-      <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[csv] - [`compareExtended(var,profile,expected,actual)`]: "list" column cell can also combine with "trim-first" (via `[profile].compareExt.matchAutoTrim`) and "insensitively compare" (via `[profile].compareExt.matchCaseInsensitive`).
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_io.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_io.data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D9B747-47F8-6143-987F-D52231B2D4E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4568A949-2BBB-B248-A980-D9837F170973}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="10520" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>true</t>
   </si>
@@ -217,9 +217,6 @@
     <t>compare1.compareExt.matchAutoTrim</t>
   </si>
   <si>
-    <t>Frin</t>
-  </si>
-  <si>
     <t>compare1.compareExt.matchAsUnorderedList</t>
   </si>
   <si>
@@ -239,6 +236,18 @@
   </si>
   <si>
     <t>index,Agg,Frin,Groups,Location,Set,Description,Amt,Units,X,4X,Curr,Rate,Subtotal</t>
+  </si>
+  <si>
+    <t>compare1.compareExt.matchAsOrderedList</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Frin,Description,Groups</t>
+  </si>
+  <si>
+    <t>Frin,Groups</t>
   </si>
 </sst>
 </file>
@@ -1893,7 +1902,7 @@
   <dimension ref="A1:AAA30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17"/>
@@ -1941,52 +1950,59 @@
         <v>46</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703" ht="23" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703" ht="23" customHeight="1">
       <c r="A7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703" ht="23" customHeight="1">
       <c r="A8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
-    <row r="9" spans="1:703" ht="23" customHeight="1"/>
+    <row r="9" spans="1:703" ht="23" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="10" spans="1:703" ht="23" customHeight="1"/>
     <row r="11" spans="1:703" ht="23" customHeight="1"/>
     <row r="12" spans="1:703" ht="23" customHeight="1"/>

</xml_diff>

<commit_message>
- Added **NEW** command line option [`-subplan`](../userguide/BatchFiles#nexial) to execute specific worksheets/subplans of a test plan for single plan execution. - [`nexial.subplansIncluded`]: **NEW** variable provides all worksheets/subplans executed by Nexial single plan execution. - [`nexial.subplansOmitted`]: **NEW** variable provides all worksheets/subplans omitted(not executed) by Nexial single plan execution.
Signed-off-by: akshay2409 <koreakshaykumar@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_io.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_io.data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nexial-Project\git\nexial-core\src\test\resources\unittesting\artifact\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4568A949-2BBB-B248-A980-D9837F170973}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="10520" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="51195" windowHeight="10515" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -38,10 +37,10 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -56,17 +55,26 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={53CD440D-8BE8-A646-9E12-01222352B648}</author>
   </authors>
   <commentList>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{53CD440D-8BE8-A646-9E12-01222352B648}">
+    <comment ref="B9" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Must explicitly use $(syspath) here so that Nexial can recognize these data variables as file paths</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -74,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
   <si>
     <t>true</t>
   </si>
@@ -97,9 +105,6 @@
     <t>filter1 fixture file</t>
   </si>
   <si>
-    <t>filter1 expected file</t>
-  </si>
-  <si>
     <t>filter1 filter</t>
   </si>
   <si>
@@ -130,9 +135,6 @@
     <t>$(syspath|data|fullpath)/unitTest_io_filter1_fixture.txt</t>
   </si>
   <si>
-    <t>$(syspath|data|fullpath)/unitTest_io_filter1_expected.txt</t>
-  </si>
-  <si>
     <t>fileDirectory</t>
   </si>
   <si>
@@ -248,12 +250,24 @@
   </si>
   <si>
     <t>Frin,Groups</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/unitTest_io_filter1_win_expected.txt</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/unitTest_io_filter1_linux_expected.txt</t>
+  </si>
+  <si>
+    <t>filter1 expected win file</t>
+  </si>
+  <si>
+    <t>filter1 expected linux file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7">
     <font>
       <sz val="12"/>
@@ -380,44 +394,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="60">
     <dxf>
       <font>
         <b val="0"/>
@@ -550,6 +527,43 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -643,6 +657,43 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -708,43 +759,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -773,43 +787,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -875,6 +852,43 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -968,6 +982,43 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1028,6 +1079,34 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1398,25 +1477,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AAA64"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="56.83203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="27.875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="56.875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
-    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+    <col min="10" max="27" width="21.125" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.875" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:703" ht="23" customHeight="1">
+    <row r="1" spans="1:703" ht="23.1" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1424,9 +1503,9 @@
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
-    <row r="2" spans="1:703" ht="23" customHeight="1">
+    <row r="2" spans="1:703" ht="23.1" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -1434,9 +1513,9 @@
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
-    <row r="3" spans="1:703" ht="23" customHeight="1">
+    <row r="3" spans="1:703" ht="23.1" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -1444,9 +1523,9 @@
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
     </row>
-    <row r="4" spans="1:703" ht="23" customHeight="1">
+    <row r="4" spans="1:703" ht="23.1" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -1454,9 +1533,9 @@
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
-    <row r="5" spans="1:703" ht="23" customHeight="1">
+    <row r="5" spans="1:703" ht="23.1" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -1464,9 +1543,9 @@
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
-    <row r="6" spans="1:703" ht="23" customHeight="1">
+    <row r="6" spans="1:703" ht="23.1" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
@@ -1474,9 +1553,9 @@
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
-    <row r="7" spans="1:703" ht="23" customHeight="1">
+    <row r="7" spans="1:703" ht="23.1" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>0</v>
@@ -1484,115 +1563,144 @@
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
-    <row r="8" spans="1:703" ht="23" customHeight="1">
+    <row r="8" spans="1:703" ht="23.1" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
-    <row r="9" spans="1:703" ht="23" customHeight="1">
+    <row r="9" spans="1:703" ht="23.1" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>
-    <row r="10" spans="1:703" ht="23" customHeight="1">
+    <row r="10" spans="1:703" ht="23.1" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>9</v>
+        <v>59</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="HA10" s="4"/>
       <c r="AAA10" s="5"/>
     </row>
-    <row r="11" spans="1:703" ht="23" customHeight="1">
-      <c r="B11" s="3"/>
+    <row r="11" spans="1:703" ht="23.1" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="HA11" s="4"/>
       <c r="AAA11" s="5"/>
     </row>
-    <row r="12" spans="1:703" ht="23" customHeight="1">
+    <row r="12" spans="1:703" ht="23.1" customHeight="1">
+      <c r="B12" s="3"/>
       <c r="HA12" s="4"/>
       <c r="AAA12" s="5"/>
     </row>
-    <row r="13" spans="1:703" ht="23" customHeight="1"/>
-    <row r="14" spans="1:703" ht="23" customHeight="1"/>
-    <row r="15" spans="1:703" ht="23" customHeight="1"/>
-    <row r="16" spans="1:703" ht="23" customHeight="1"/>
-    <row r="17" ht="23" customHeight="1"/>
-    <row r="18" ht="23" customHeight="1"/>
-    <row r="19" ht="23" customHeight="1"/>
-    <row r="20" ht="23" customHeight="1"/>
-    <row r="21" ht="23" customHeight="1"/>
-    <row r="22" ht="23" customHeight="1"/>
-    <row r="23" ht="23" customHeight="1"/>
-    <row r="24" ht="23" customHeight="1"/>
-    <row r="25" ht="23" customHeight="1"/>
-    <row r="26" ht="23" customHeight="1"/>
-    <row r="27" ht="23" customHeight="1"/>
-    <row r="28" ht="23" customHeight="1"/>
-    <row r="29" ht="23" customHeight="1"/>
-    <row r="30" ht="23" customHeight="1"/>
-    <row r="31" ht="23" customHeight="1"/>
-    <row r="32" ht="23" customHeight="1"/>
-    <row r="33" ht="23" customHeight="1"/>
-    <row r="34" ht="23" customHeight="1"/>
-    <row r="35" ht="23" customHeight="1"/>
-    <row r="36" ht="23" customHeight="1"/>
-    <row r="37" ht="23" customHeight="1"/>
-    <row r="38" ht="23" customHeight="1"/>
-    <row r="39" ht="23" customHeight="1"/>
-    <row r="40" ht="23" customHeight="1"/>
-    <row r="41" ht="23" customHeight="1"/>
-    <row r="42" ht="23" customHeight="1"/>
-    <row r="43" ht="23" customHeight="1"/>
-    <row r="44" ht="23" customHeight="1"/>
-    <row r="45" ht="23" customHeight="1"/>
-    <row r="46" ht="23" customHeight="1"/>
-    <row r="47" ht="23" customHeight="1"/>
-    <row r="48" ht="23" customHeight="1"/>
-    <row r="49" ht="23" customHeight="1"/>
-    <row r="50" ht="23" customHeight="1"/>
-    <row r="51" ht="23" customHeight="1"/>
-    <row r="52" ht="23" customHeight="1"/>
-    <row r="53" ht="23" customHeight="1"/>
-    <row r="54" ht="23" customHeight="1"/>
-    <row r="55" ht="23" customHeight="1"/>
-    <row r="56" ht="23" customHeight="1"/>
-    <row r="57" ht="23" customHeight="1"/>
-    <row r="58" ht="23" customHeight="1"/>
-    <row r="59" ht="23" customHeight="1"/>
-    <row r="60" ht="23" customHeight="1"/>
-    <row r="61" ht="23" customHeight="1"/>
-    <row r="62" ht="23" customHeight="1"/>
-    <row r="63" ht="23" customHeight="1"/>
+    <row r="13" spans="1:703" ht="23.1" customHeight="1">
+      <c r="HA13" s="4"/>
+      <c r="AAA13" s="5"/>
+    </row>
+    <row r="14" spans="1:703" ht="23.1" customHeight="1"/>
+    <row r="15" spans="1:703" ht="23.1" customHeight="1"/>
+    <row r="16" spans="1:703" ht="23.1" customHeight="1"/>
+    <row r="17" ht="23.1" customHeight="1"/>
+    <row r="18" ht="23.1" customHeight="1"/>
+    <row r="19" ht="23.1" customHeight="1"/>
+    <row r="20" ht="23.1" customHeight="1"/>
+    <row r="21" ht="23.1" customHeight="1"/>
+    <row r="22" ht="23.1" customHeight="1"/>
+    <row r="23" ht="23.1" customHeight="1"/>
+    <row r="24" ht="23.1" customHeight="1"/>
+    <row r="25" ht="23.1" customHeight="1"/>
+    <row r="26" ht="23.1" customHeight="1"/>
+    <row r="27" ht="23.1" customHeight="1"/>
+    <row r="28" ht="23.1" customHeight="1"/>
+    <row r="29" ht="23.1" customHeight="1"/>
+    <row r="30" ht="23.1" customHeight="1"/>
+    <row r="31" ht="23.1" customHeight="1"/>
+    <row r="32" ht="23.1" customHeight="1"/>
+    <row r="33" ht="23.1" customHeight="1"/>
+    <row r="34" ht="23.1" customHeight="1"/>
+    <row r="35" ht="23.1" customHeight="1"/>
+    <row r="36" ht="23.1" customHeight="1"/>
+    <row r="37" ht="23.1" customHeight="1"/>
+    <row r="38" ht="23.1" customHeight="1"/>
+    <row r="39" ht="23.1" customHeight="1"/>
+    <row r="40" ht="23.1" customHeight="1"/>
+    <row r="41" ht="23.1" customHeight="1"/>
+    <row r="42" ht="23.1" customHeight="1"/>
+    <row r="43" ht="23.1" customHeight="1"/>
+    <row r="44" ht="23.1" customHeight="1"/>
+    <row r="45" ht="23.1" customHeight="1"/>
+    <row r="46" ht="23.1" customHeight="1"/>
+    <row r="47" ht="23.1" customHeight="1"/>
+    <row r="48" ht="23.1" customHeight="1"/>
+    <row r="49" ht="23.1" customHeight="1"/>
+    <row r="50" ht="23.1" customHeight="1"/>
+    <row r="51" ht="23.1" customHeight="1"/>
+    <row r="52" ht="23.1" customHeight="1"/>
+    <row r="53" ht="23.1" customHeight="1"/>
+    <row r="54" ht="23.1" customHeight="1"/>
+    <row r="55" ht="23.1" customHeight="1"/>
+    <row r="56" ht="23.1" customHeight="1"/>
+    <row r="57" ht="23.1" customHeight="1"/>
+    <row r="58" ht="23.1" customHeight="1"/>
+    <row r="59" ht="23.1" customHeight="1"/>
+    <row r="60" ht="23.1" customHeight="1"/>
+    <row r="61" ht="23.1" customHeight="1"/>
+    <row r="62" ht="23.1" customHeight="1"/>
+    <row r="63" ht="23.1" customHeight="1"/>
+    <row r="64" ht="23.1" customHeight="1"/>
   </sheetData>
-  <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="54" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A1:A8 A10:A1048576">
+    <cfRule type="beginsWith" dxfId="9" priority="11" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="53" priority="7" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="8" priority="12" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="52" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="13" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B9 B12:B1048576">
-    <cfRule type="expression" dxfId="51" priority="9" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B8 B13:B1048576 B10">
+    <cfRule type="expression" dxfId="6" priority="14" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="50" priority="10">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="15">
       <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9">
+    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A9,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A9,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
+      <formula>LEN(TRIM(A9))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
+      <formula>LEN(TRIM(B9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1601,26 +1709,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56E3E307-7F2E-46DB-89A3-7D5088FF1029}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AAA30"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="27.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="27.875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="84" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.125" style="3" customWidth="1" collapsed="1"/>
     <col min="4" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
-    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+    <col min="10" max="27" width="21.125" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.875" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:703" ht="23" customHeight="1">
+    <row r="1" spans="1:703" ht="23.1" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1628,9 +1736,9 @@
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
-    <row r="2" spans="1:703" ht="23" customHeight="1">
+    <row r="2" spans="1:703" ht="23.1" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -1638,9 +1746,9 @@
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
-    <row r="3" spans="1:703" ht="23" customHeight="1">
+    <row r="3" spans="1:703" ht="23.1" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
@@ -1648,19 +1756,19 @@
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
     </row>
-    <row r="4" spans="1:703" ht="23" customHeight="1">
+    <row r="4" spans="1:703" ht="23.1" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
-    <row r="5" spans="1:703" ht="23" customHeight="1">
+    <row r="5" spans="1:703" ht="23.1" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -1668,9 +1776,9 @@
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
-    <row r="6" spans="1:703" ht="23" customHeight="1">
+    <row r="6" spans="1:703" ht="23.1" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
@@ -1678,9 +1786,9 @@
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
-    <row r="7" spans="1:703" ht="23" customHeight="1">
+    <row r="7" spans="1:703" ht="23.1" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>0</v>
@@ -1688,206 +1796,206 @@
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
-    <row r="8" spans="1:703" ht="23" customHeight="1">
+    <row r="8" spans="1:703" ht="23.1" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
-    <row r="9" spans="1:703" ht="23" customHeight="1">
+    <row r="9" spans="1:703" ht="23.1" customHeight="1">
       <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:703" ht="23.1" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:703" ht="23.1" customHeight="1">
+      <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:703" ht="23" customHeight="1">
-      <c r="A10" s="1" t="s">
+    <row r="12" spans="1:703" ht="23.1" customHeight="1">
+      <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:703" ht="23" customHeight="1">
-      <c r="A11" s="1" t="s">
+      <c r="B12" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:703" ht="23.1" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:703" ht="23" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:703" ht="23" customHeight="1">
-      <c r="A13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="HA13" s="4"/>
       <c r="AAA13" s="5"/>
     </row>
-    <row r="14" spans="1:703" ht="23" customHeight="1">
+    <row r="14" spans="1:703" ht="23.1" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="HA14" s="4"/>
       <c r="AAA14" s="5"/>
     </row>
-    <row r="15" spans="1:703" ht="23" customHeight="1">
+    <row r="15" spans="1:703" ht="23.1" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:703" ht="23" customHeight="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:703" ht="23.1" customHeight="1">
       <c r="A16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="23.1" customHeight="1">
+      <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="23" customHeight="1">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:2" ht="23.1" customHeight="1">
+      <c r="A18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="23" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="23" customHeight="1"/>
-    <row r="20" spans="1:2" ht="23" customHeight="1"/>
-    <row r="21" spans="1:2" ht="23" customHeight="1"/>
-    <row r="22" spans="1:2" ht="23" customHeight="1"/>
-    <row r="23" spans="1:2" ht="23" customHeight="1"/>
-    <row r="24" spans="1:2" ht="23" customHeight="1"/>
-    <row r="25" spans="1:2" ht="23" customHeight="1"/>
-    <row r="26" spans="1:2" ht="23" customHeight="1"/>
-    <row r="27" spans="1:2" ht="23" customHeight="1"/>
-    <row r="28" spans="1:2" ht="23" customHeight="1"/>
-    <row r="29" spans="1:2" ht="23" customHeight="1"/>
-    <row r="30" spans="1:2" ht="23" customHeight="1"/>
+    </row>
+    <row r="19" spans="1:2" ht="23.1" customHeight="1"/>
+    <row r="20" spans="1:2" ht="23.1" customHeight="1"/>
+    <row r="21" spans="1:2" ht="23.1" customHeight="1"/>
+    <row r="22" spans="1:2" ht="23.1" customHeight="1"/>
+    <row r="23" spans="1:2" ht="23.1" customHeight="1"/>
+    <row r="24" spans="1:2" ht="23.1" customHeight="1"/>
+    <row r="25" spans="1:2" ht="23.1" customHeight="1"/>
+    <row r="26" spans="1:2" ht="23.1" customHeight="1"/>
+    <row r="27" spans="1:2" ht="23.1" customHeight="1"/>
+    <row r="28" spans="1:2" ht="23.1" customHeight="1"/>
+    <row r="29" spans="1:2" ht="23.1" customHeight="1"/>
+    <row r="30" spans="1:2" ht="23.1" customHeight="1"/>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A19:A1048576 A13:A15 A1:A8 A17">
-    <cfRule type="beginsWith" dxfId="49" priority="24" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="59" priority="24" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="48" priority="25" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="58" priority="25" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="47" priority="26" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="57" priority="26" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B15 B19:B1048576 B1:B8 B17">
-    <cfRule type="expression" dxfId="46" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="27" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="45" priority="28">
+    <cfRule type="notContainsBlanks" dxfId="55" priority="28">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="44" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="22" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="43" priority="23">
+    <cfRule type="notContainsBlanks" dxfId="53" priority="23">
       <formula>LEN(TRIM(B18))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:A11">
-    <cfRule type="beginsWith" dxfId="42" priority="14" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="52" priority="14" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A9,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="41" priority="15" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="51" priority="15" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A9,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="40" priority="16" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(A9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:B11">
-    <cfRule type="expression" dxfId="39" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="17" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="38" priority="18">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="18">
       <formula>LEN(TRIM(B9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="beginsWith" dxfId="37" priority="9" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="47" priority="9" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A12,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="36" priority="10" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="46" priority="10" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A12,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="35" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="34" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="33" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="13">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="beginsWith" dxfId="32" priority="4" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="42" priority="4" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A16,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="31" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="41" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A16,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="30" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="29" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="28" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="8">
       <formula>LEN(TRIM(B16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18">
-    <cfRule type="beginsWith" dxfId="27" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="37" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A18,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="26" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="36" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A18,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="25" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A18))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1898,46 +2006,46 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38ED455C-CA2D-0146-BE90-42ACB3222138}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AAA30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="39.625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="84" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.125" style="3" customWidth="1" collapsed="1"/>
     <col min="4" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
-    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+    <col min="10" max="27" width="21.125" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.875" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:703" ht="23" customHeight="1">
+    <row r="1" spans="1:703" ht="23.1" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
-    <row r="2" spans="1:703" ht="23" customHeight="1">
+    <row r="2" spans="1:703" ht="23.1" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
-    <row r="3" spans="1:703" ht="23" customHeight="1">
+    <row r="3" spans="1:703" ht="23.1" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -1945,187 +2053,187 @@
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
     </row>
-    <row r="4" spans="1:703" ht="23" customHeight="1">
+    <row r="4" spans="1:703" ht="23.1" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
-    <row r="5" spans="1:703" ht="23" customHeight="1">
+    <row r="5" spans="1:703" ht="23.1" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
-    <row r="6" spans="1:703" ht="23" customHeight="1">
+    <row r="6" spans="1:703" ht="23.1" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
-    <row r="7" spans="1:703" ht="23" customHeight="1">
+    <row r="7" spans="1:703" ht="23.1" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
-    <row r="8" spans="1:703" ht="23" customHeight="1">
+    <row r="8" spans="1:703" ht="23.1" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
-    <row r="9" spans="1:703" ht="23" customHeight="1">
+    <row r="9" spans="1:703" ht="23.1" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:703" ht="23" customHeight="1"/>
-    <row r="11" spans="1:703" ht="23" customHeight="1"/>
-    <row r="12" spans="1:703" ht="23" customHeight="1"/>
-    <row r="13" spans="1:703" ht="23" customHeight="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:703" ht="23.1" customHeight="1"/>
+    <row r="11" spans="1:703" ht="23.1" customHeight="1"/>
+    <row r="12" spans="1:703" ht="23.1" customHeight="1"/>
+    <row r="13" spans="1:703" ht="23.1" customHeight="1">
       <c r="B13" s="3"/>
       <c r="HA13" s="4"/>
       <c r="AAA13" s="5"/>
     </row>
-    <row r="14" spans="1:703" ht="23" customHeight="1">
+    <row r="14" spans="1:703" ht="23.1" customHeight="1">
       <c r="B14" s="7"/>
       <c r="HA14" s="4"/>
       <c r="AAA14" s="5"/>
     </row>
-    <row r="15" spans="1:703" ht="23" customHeight="1"/>
-    <row r="16" spans="1:703" ht="23" customHeight="1"/>
-    <row r="17" ht="23" customHeight="1"/>
-    <row r="18" ht="23" customHeight="1"/>
-    <row r="19" ht="23" customHeight="1"/>
-    <row r="20" ht="23" customHeight="1"/>
-    <row r="21" ht="23" customHeight="1"/>
-    <row r="22" ht="23" customHeight="1"/>
-    <row r="23" ht="23" customHeight="1"/>
-    <row r="24" ht="23" customHeight="1"/>
-    <row r="25" ht="23" customHeight="1"/>
-    <row r="26" ht="23" customHeight="1"/>
-    <row r="27" ht="23" customHeight="1"/>
-    <row r="28" ht="23" customHeight="1"/>
-    <row r="29" ht="23" customHeight="1"/>
-    <row r="30" ht="23" customHeight="1"/>
+    <row r="15" spans="1:703" ht="23.1" customHeight="1"/>
+    <row r="16" spans="1:703" ht="23.1" customHeight="1"/>
+    <row r="17" ht="23.1" customHeight="1"/>
+    <row r="18" ht="23.1" customHeight="1"/>
+    <row r="19" ht="23.1" customHeight="1"/>
+    <row r="20" ht="23.1" customHeight="1"/>
+    <row r="21" ht="23.1" customHeight="1"/>
+    <row r="22" ht="23.1" customHeight="1"/>
+    <row r="23" ht="23.1" customHeight="1"/>
+    <row r="24" ht="23.1" customHeight="1"/>
+    <row r="25" ht="23.1" customHeight="1"/>
+    <row r="26" ht="23.1" customHeight="1"/>
+    <row r="27" ht="23.1" customHeight="1"/>
+    <row r="28" ht="23.1" customHeight="1"/>
+    <row r="29" ht="23.1" customHeight="1"/>
+    <row r="30" ht="23.1" customHeight="1"/>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A19:A1048576 A13:A15 A1:A8 A17">
-    <cfRule type="beginsWith" dxfId="24" priority="21" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="34" priority="21" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="23" priority="22" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="33" priority="22" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="22" priority="23" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="23" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B15 B19:B1048576 B1:B8 B17">
-    <cfRule type="expression" dxfId="21" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="24" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="20" priority="25">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="25">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="19" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="18" priority="20">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="20">
       <formula>LEN(TRIM(B18))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:A11">
-    <cfRule type="beginsWith" dxfId="17" priority="14" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="27" priority="14" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A9,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="16" priority="15" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="26" priority="15" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A9,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="15" priority="16" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(A9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:B11">
-    <cfRule type="expression" dxfId="14" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="17" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="13" priority="18">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="18">
       <formula>LEN(TRIM(B9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="beginsWith" dxfId="12" priority="9" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="22" priority="9" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A12,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="11" priority="10" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="21" priority="10" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A12,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="11" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="11" stopIfTrue="1">
       <formula>LEN(TRIM(A12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="9" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="12" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="8" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="13">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="beginsWith" dxfId="7" priority="4" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="17" priority="4" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A16,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="6" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="16" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A16,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="6" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="3" priority="8">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="8">
       <formula>LEN(TRIM(B16))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18">
-    <cfRule type="beginsWith" dxfId="2" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="12" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A18,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="11" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A18,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A18))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>